<commit_message>
Changed path to TomLeversRPackage in R command. perform_Box_Cox_Method provides transformed predictor values. Completed homework for Model Diagnostics and Remedial Measures in SLR.
Going to start first project for Linear Models
</commit_message>
<xml_diff>
--- a/R/R_Commands.xlsx
+++ b/R/R_Commands.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Documents\Tom_Levers_Git_Repository\TomLeversRPackage\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Documents\Tom_Levers_Git_Repository\R\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{940EC38D-6F39-419C-8AC6-B0CE888AF5F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05D206EF-D099-41E0-B0C4-C73B41541587}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8700" yWindow="2530" windowWidth="28800" windowHeight="15470" xr2:uid="{4113E9C0-2B3F-A842-BEAE-53D8B59B8F27}"/>
+    <workbookView xWindow="130" yWindow="3920" windowWidth="18910" windowHeight="15470" xr2:uid="{4113E9C0-2B3F-A842-BEAE-53D8B59B8F27}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -125,14 +125,14 @@
     <t>Updated: 09/14/22 by Tom Lever</t>
   </si>
   <si>
+    <t>Restart R session</t>
+  </si>
+  <si>
+    <t>.rs.restartR()</t>
+  </si>
+  <si>
     <t>install.packages("tidyverse", repos = "http://cran.us.r-project.org")
-install.packages("C:\\Users\\Tom\\Documents\\Tom_Levers_Git_Repository\\TomLeversRPackage", repos = NULL, type="source")</t>
-  </si>
-  <si>
-    <t>Restart R session</t>
-  </si>
-  <si>
-    <t>.rs.restartR()</t>
+install.packages("C:\\Users\\Tom\\Documents\\Tom_Levers_Git_Repository\\R\\TomLeversRPackage", repos = NULL, type="source")</t>
   </si>
 </sst>
 </file>
@@ -514,7 +514,7 @@
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="34.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="109" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="111.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="26" x14ac:dyDescent="0.6">
@@ -577,7 +577,7 @@
         <v>5</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
@@ -606,10 +606,10 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" t="s">
         <v>31</v>
-      </c>
-      <c r="B15" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Created calculate_PRESS. Completed Guided Question Set for Model Selection through using calculate_PRESS
Going to calculate {R_{prediction}}^2 and R^2 for y ~ x2 + x7 + x8
</commit_message>
<xml_diff>
--- a/R/R_Commands.xlsx
+++ b/R/R_Commands.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Documents\Tom_Levers_Git_Repository\R\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05D206EF-D099-41E0-B0C4-C73B41541587}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0E6A613-31F0-4AF0-BECE-FB6176E472E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="130" yWindow="3920" windowWidth="18910" windowHeight="15470" xr2:uid="{4113E9C0-2B3F-A842-BEAE-53D8B59B8F27}"/>
+    <workbookView xWindow="40" yWindow="80" windowWidth="22120" windowHeight="20730" xr2:uid="{4113E9C0-2B3F-A842-BEAE-53D8B59B8F27}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -131,8 +131,8 @@
     <t>.rs.restartR()</t>
   </si>
   <si>
-    <t>install.packages("tidyverse", repos = "http://cran.us.r-project.org")
-install.packages("C:\\Users\\Tom\\Documents\\Tom_Levers_Git_Repository\\R\\TomLeversRPackage", repos = NULL, type="source")</t>
+    <t>install.packages("C:\\Users\\Tom\\Documents\\Tom_Levers_Git_Repository\\R\\TomLeversRPackage", repos = NULL, type="source")
+install.packages("tidyverse", repos = "http://cran.us.r-project.org")</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Added command for installing TomLeversRPackage on Mac. Exported calculate residual mean square. Allowed declaring reference class in convert_to_categorical_vector. Created summarize_all_MLR_models.
Going to parallel Introduction to Linear Regression Analysis, 10.2: Computational Techniques for Variable Selection, 10.2.1: All Possible Regressions, Example 10.1: The Hald Cement Data for Studying The Age And Sex of Abalones.
</commit_message>
<xml_diff>
--- a/R/R_Commands.xlsx
+++ b/R/R_Commands.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Documents\Tom_Levers_Git_Repository\R\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tlever/Tom_Levers_Git_Repository/R/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0E6A613-31F0-4AF0-BECE-FB6176E472E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC532F6B-6359-A744-BC24-FD3008779FAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40" yWindow="80" windowWidth="22120" windowHeight="20730" xr2:uid="{4113E9C0-2B3F-A842-BEAE-53D8B59B8F27}"/>
+    <workbookView xWindow="40" yWindow="760" windowWidth="22120" windowHeight="19880" xr2:uid="{4113E9C0-2B3F-A842-BEAE-53D8B59B8F27}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -132,6 +132,7 @@
   </si>
   <si>
     <t>install.packages("C:\\Users\\Tom\\Documents\\Tom_Levers_Git_Repository\\R\\TomLeversRPackage", repos = NULL, type="source")
+install.packages("/Users/tlever/Tom_Levers_Git_Repository/R/TomLeversRPackage", repos = NULL, type="source")
 install.packages("tidyverse", repos = "http://cran.us.r-project.org")</t>
   </si>
 </sst>
@@ -511,28 +512,28 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="34.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="111.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="26" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:2" ht="26" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
@@ -540,7 +541,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -548,7 +549,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -556,7 +557,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -564,7 +565,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -572,7 +573,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="31" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" ht="68" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -580,7 +581,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -588,7 +589,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -596,7 +597,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -604,7 +605,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>30</v>
       </c>
@@ -612,7 +613,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -620,7 +621,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -628,7 +629,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>11</v>
       </c>
@@ -636,7 +637,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>13</v>
       </c>
@@ -644,7 +645,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>15</v>
       </c>

</xml_diff>